<commit_message>
updated seeds & minor fixes
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\AnacondaProjects\kaggle_COMPETITIONS\moa_kaggle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757E5261-7F32-4500-8FB1-EF89EAD46ABE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3864755-EFE1-4427-BE45-0863FC545EA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -167,9 +167,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -182,10 +179,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,16 +483,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -518,7 +518,7 @@
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C3">
@@ -527,7 +527,7 @@
       <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G3">
@@ -538,7 +538,7 @@
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C4">
@@ -547,7 +547,7 @@
       <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G4">
@@ -558,7 +558,7 @@
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C5">
@@ -567,7 +567,7 @@
       <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G5">
@@ -578,7 +578,7 @@
       <c r="E6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="G6">
@@ -589,55 +589,55 @@
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="E8" s="8" t="s">
+      <c r="B8" s="9"/>
+      <c r="E8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>256</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>1E-3</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>128</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>1.6E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="6"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E13" t="s">

</xml_diff>